<commit_message>
Update capacitiveTouch sensor cost
</commit_message>
<xml_diff>
--- a/capacitiveTouchRelay/Cost.xlsx
+++ b/capacitiveTouchRelay/Cost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="6120" windowWidth="13420" windowHeight="19280" tabRatio="500"/>
+    <workbookView xWindow="3720" yWindow="320" windowWidth="23980" windowHeight="26340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>white breadboard</t>
   </si>
@@ -84,13 +84,16 @@
     <t>Mechanical Components</t>
   </si>
   <si>
-    <t>Time (hr)</t>
-  </si>
-  <si>
     <t>Electrical Components</t>
   </si>
   <si>
     <t>Shipping</t>
+  </si>
+  <si>
+    <t>Time (hr). Took 8 hrs. 1hr to prepare, 4hrs to implement, 3hrs to clean up and document. I quoted you for 5hrs so will only charge that.</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,8 +158,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -176,8 +194,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
@@ -185,12 +211,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -200,6 +230,10 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -209,6 +243,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,7 +579,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D28" sqref="A1:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -550,6 +588,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
+      <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
@@ -561,297 +600,341 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>25.81</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
         <f>C3*B3</f>
         <v>25.81</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>1.5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <f t="shared" ref="D4:D11" si="0">C4*B4</f>
         <v>1.5</v>
       </c>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
         <v>4.67</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
         <f t="shared" si="0"/>
         <v>4.67</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>5.4</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="30">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>0.5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>0</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>3.4</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
         <f t="shared" ref="D14:D20" si="1">C14*B14</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>0.1</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>0.1</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <v>0.1</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>0.4</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>0.5</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>1.86</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
+    <row r="21" spans="1:4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="75">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <f t="shared" ref="D22" si="2">C22*B22</f>
         <v>250</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+    </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
         <v>16.350000000000001</v>
       </c>
     </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+    </row>
     <row r="28" spans="1:4">
-      <c r="D28">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="6">
         <f>SUM(D3:D27)</f>
         <v>318.19</v>
       </c>

</xml_diff>